<commit_message>
renamed app - doug to app (after deleting app folder). Minor updates. creation of power point and word docs
</commit_message>
<xml_diff>
--- a/app/data/Application Performance Score Card.xlsx
+++ b/app/data/Application Performance Score Card.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougi\GitHub\AI_Course_Project_3_Team_1\app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dougi\GitHub\AI_Course_Project_3_Team_1\app - Doug\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D18C46C-B163-4B50-9AAB-0C7D4173C271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A700CEA-45E6-4713-B296-AF7DFC26CFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25815" yWindow="11130" windowWidth="21600" windowHeight="10920" xr2:uid="{20BB431B-6E89-477C-866D-A5B7D66F952A}"/>
+    <workbookView xWindow="-28920" yWindow="9315" windowWidth="29040" windowHeight="15720" xr2:uid="{20BB431B-6E89-477C-866D-A5B7D66F952A}"/>
   </bookViews>
   <sheets>
     <sheet name="Graphing Request Score Card" sheetId="1" r:id="rId1"/>
@@ -217,7 +217,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -458,26 +458,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -507,14 +495,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -853,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06800544-4F76-46AE-927E-27A17DA18F7B}">
   <dimension ref="A2:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -867,29 +864,29 @@
   <sheetData>
     <row r="2" spans="1:4" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="3" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:4" ht="18.3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -898,12 +895,12 @@
       <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="94.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -912,12 +909,12 @@
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="7" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -926,10 +923,10 @@
       <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="11"/>
+      <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -938,12 +935,12 @@
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -952,10 +949,10 @@
       <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="13"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -964,10 +961,10 @@
       <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="11"/>
-    </row>
-    <row r="11" spans="1:4" ht="93.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="12" t="s">
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" ht="59.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -976,68 +973,68 @@
       <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="54.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1046,12 +1043,12 @@
       <c r="C16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1060,12 +1057,12 @@
       <c r="C17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="93.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1074,12 +1071,12 @@
       <c r="C18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="93.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1088,12 +1085,12 @@
       <c r="C19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="7" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="93.6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1102,12 +1099,12 @@
       <c r="C20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1116,12 +1113,12 @@
       <c r="C21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1130,12 +1127,12 @@
       <c r="C22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1144,10 +1141,10 @@
       <c r="C23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="11"/>
+      <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1156,10 +1153,10 @@
       <c r="C24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="11"/>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1168,10 +1165,10 @@
       <c r="C25" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="11"/>
+      <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1180,21 +1177,21 @@
       <c r="C26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="12" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1202,35 +1199,35 @@
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="19">
+      <c r="B31" s="15">
         <f>20/23</f>
         <v>0.86956521739130432</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="16" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="20">
+      <c r="B33" s="16">
         <f>19/20</f>
         <v>0.95</v>
       </c>

</xml_diff>